<commit_message>
Update excel file example
</commit_message>
<xml_diff>
--- a/OfficeAddIns/ExcelAddIns/BananaAccounting/BananaAccountingExcelAddin_example.xlsx
+++ b/OfficeAddIns/ExcelAddIns/BananaAccounting/BananaAccountingExcelAddin_example.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Documents/GitHub/General/OfficeAddIns/ExcelAddIns/BananaAccounting/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23610" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23620" windowHeight="10700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -308,7 +314,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -818,7 +824,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="1" width="700" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -842,20 +848,20 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="13.73046875" customWidth="1"/>
-    <col min="5" max="5" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.73046875" customWidth="1"/>
-    <col min="11" max="12" width="11.73046875" customWidth="1"/>
+    <col min="1" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -863,7 +869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -871,7 +877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -891,7 +897,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -911,22 +917,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -937,7 +943,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -948,7 +954,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -971,7 +977,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1086,7 +1092,7 @@
       <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1139,7 +1145,7 @@
       <c r="AX16" s="1"/>
       <c r="AY16" s="1"/>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1195,7 +1201,7 @@
       <c r="AX17" s="1"/>
       <c r="AY17" s="1"/>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1251,7 +1257,7 @@
       <c r="AX18" s="1"/>
       <c r="AY18" s="1"/>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1306,7 +1312,7 @@
       <c r="AX19" s="1"/>
       <c r="AY19" s="1"/>
     </row>
-    <row r="20" spans="1:51" ht="21" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:51" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1361,7 +1367,7 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1426,7 +1432,7 @@
       <c r="AX21" s="1"/>
       <c r="AY21" s="1"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>1657 %</v>
       </c>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>42.7 %</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>100 %</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:51" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>130.7 %</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="28" spans="1:51" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:51" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="30" spans="1:51" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:51" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1722,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="32" spans="1:51" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:51" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>69 %</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -2006,7 +2012,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>0 %</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>44</v>
       </c>
@@ -2064,12 +2070,12 @@
         <v>14.6 %</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
     </row>
-    <row r="45" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="F45" s="10">
         <f>F9</f>
@@ -2089,7 +2095,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>-133.4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2147,7 +2153,7 @@
         <v>-155.19999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>-138.79999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="5" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>-231.4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>55</v>
       </c>

</xml_diff>